<commit_message>
Update binary files for labeling and survey parser
</commit_message>
<xml_diff>
--- a/data/children_labeling.xlsx
+++ b/data/children_labeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Stav\vscode\ema-pipeline\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9899334C-4305-437B-BE2D-1E58598049B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3056E786-3CC6-456B-A227-5EEE480641B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA231A5-A2FD-4520-B05B-38B600A13544}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
   <si>
     <t>hebrew_text</t>
   </si>
@@ -44,9 +44,6 @@
     <t>hebrew_option</t>
   </si>
   <si>
-    <t>variable_name</t>
-  </si>
-  <si>
     <t>ברגע זה אני מרגיש חסר מנוחה</t>
   </si>
   <si>
@@ -89,27 +86,15 @@
     <t>צעקתי</t>
   </si>
   <si>
-    <t>C_Agr_shout</t>
-  </si>
-  <si>
     <t>טרקתי דלת</t>
   </si>
   <si>
-    <t>C_Agr_door</t>
-  </si>
-  <si>
     <t>זרקתי משהו</t>
   </si>
   <si>
-    <t>C_Agr_throw</t>
-  </si>
-  <si>
     <t>זרקתי משהו על מישהו</t>
   </si>
   <si>
-    <t>C_Agr_throw_at</t>
-  </si>
-  <si>
     <t>הרבצתי</t>
   </si>
   <si>
@@ -282,14 +267,52 @@
   </si>
   <si>
     <t>מאז הסקר האחרון, אמא שלי הסכימה לכל מה שרציתי</t>
+  </si>
+  <si>
+    <t>ברגע זה, אני מרגישה חסר מנוחה</t>
+  </si>
+  <si>
+    <t>C_Inv_Help</t>
+  </si>
+  <si>
+    <t>C_PC_Sharing</t>
+  </si>
+  <si>
+    <t>מאז הסקר האחרון, עצבנתי את אמא שלי</t>
+  </si>
+  <si>
+    <t>C_Agr_throw_smt</t>
+  </si>
+  <si>
+    <t>C_Agr_throw_twd</t>
+  </si>
+  <si>
+    <t>C_Agr_yelled</t>
+  </si>
+  <si>
+    <t>C_Agr_slam</t>
+  </si>
+  <si>
+    <t>ברגע זה, אני מרגיש טוב</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -317,13 +340,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -334,6 +364,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F3E5278-7A2A-4199-9905-1510421EA995}" name="Table1" displayName="Table1" ref="A1:C55" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C55" xr:uid="{5F3E5278-7A2A-4199-9905-1510421EA995}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{31577ADF-9116-4E61-AB6C-254022F6B686}" name="hebrew_text"/>
+    <tableColumn id="2" xr3:uid="{440EAB83-894B-4CBF-917F-73D113C57556}" name="hebrew_option"/>
+    <tableColumn id="3" xr3:uid="{A4999A05-C54E-42B4-919E-1389FAB4FE6F}" name="label"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -653,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F683BF62-4417-43F4-ADCE-01CD126760AF}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,702 +709,476 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C51" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="C52" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>35</v>
-      </c>
-      <c r="C58" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>38</v>
-      </c>
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>39</v>
-      </c>
-      <c r="C62" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>40</v>
-      </c>
-      <c r="C63" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>41</v>
-      </c>
-      <c r="C64" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>42</v>
-      </c>
-      <c r="C65" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>43</v>
-      </c>
-      <c r="C66" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>44</v>
-      </c>
-      <c r="C67" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>45</v>
-      </c>
-      <c r="C68" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>46</v>
-      </c>
-      <c r="C69" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>79</v>
-      </c>
-      <c r="C70" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>80</v>
-      </c>
-      <c r="C71" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>71</v>
-      </c>
-      <c r="C72" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>67</v>
-      </c>
-      <c r="C74" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>70</v>
-      </c>
-      <c r="C75" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>81</v>
-      </c>
-      <c r="C76" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>73</v>
-      </c>
-      <c r="C78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>75</v>
-      </c>
-      <c r="C79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>34</v>
-      </c>
-      <c r="C81" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>35</v>
-      </c>
-      <c r="C82" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>65</v>
-      </c>
-      <c r="C83" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>64</v>
-      </c>
-      <c r="C84" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C55">
+    <sortCondition ref="C2:C55"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance labeling and survey parsing functionality
- Added a `clean` function to normalize and clean Hebrew text inputs in `labeling.py`.
- Refactored `load_labeling_map` to utilize the new `clean` function for processing text.
- Updated `relabel_columns` to improve matching of question texts and handle unmatched cases.
- Simplified `parse_survey_folder` by integrating `relabel_columns` for better column mapping.
- Introduced logging for unmatched questions to `unmatched_questions.log` for easier debugging.
- Removed obsolete functions related to column matching and example column checks in `survey_parser.py`.
</commit_message>
<xml_diff>
--- a/data/children_labeling.xlsx
+++ b/data/children_labeling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Stav\vscode\ema-pipeline\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3056E786-3CC6-456B-A227-5EEE480641B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A091FA0D-18E5-4A97-87A1-F4DFAAAA14E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FA231A5-A2FD-4520-B05B-38B600A13544}"/>
+    <workbookView xWindow="15975" yWindow="2505" windowWidth="10155" windowHeight="8220" xr2:uid="{4FA231A5-A2FD-4520-B05B-38B600A13544}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>C_Anx_now</t>
   </si>
   <si>
-    <t>מאז הסקר האחרון, היה לי קשה להפסיק לעשות משהו אחרי שביקשו ממני להפסיק</t>
-  </si>
-  <si>
     <t>C_IC_CantStop</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>מאז הסקר האחרון, אבא שלי הסכים לכל מה שרציתי</t>
   </si>
   <si>
-    <t>מאז הסקר האחרון, שיתפתי את אבא שלי ברגשות/תחושות שלי</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, אבא שלי העביר עליי ביקורת</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>מאז הסקר האחרון, אבא שלי איים להעניש אותי אבל לא עשה זאת</t>
   </si>
   <si>
-    <t>היום אבא שלי עזר לי במשהו</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, הרגשתי מתוסכל</t>
   </si>
   <si>
@@ -221,9 +212,6 @@
     <t>מאז הסקר האחרון, אמא שלי החמיאה לי כשעשיתי משהו בצורה טובה</t>
   </si>
   <si>
-    <t>מאז הסקר האחרון, שיתפתי את אמא שלי ברגשות/תחושות שלי</t>
-  </si>
-  <si>
     <t>מאז הסקר האחרון, אמא שלי איימה להעניש אותי אבל לא עשתה זאת</t>
   </si>
   <si>
@@ -233,9 +221,6 @@
     <t>ברגע ,זה אני מרגיש טוב</t>
   </si>
   <si>
-    <t>היום אמא שלי עזרה לי במשהו</t>
-  </si>
-  <si>
     <t>היום אמא שלי דיברה איתי על החברים שלי או על היום שלי</t>
   </si>
   <si>
@@ -297,6 +282,21 @@
   </si>
   <si>
     <t>label</t>
+  </si>
+  <si>
+    <t>מאז הסקר האחרון, היה לי קשה להפסיק לעשות משהו אחרי שביקשו ממני להפסיק (לדוגמה כשמורים מבקשים ממני להפסיק לדבר בכיתה או כשאבא מבקש ממני להפסיק להיות מול המסך)</t>
+  </si>
+  <si>
+    <t>היום אבא שלי עזר לי במשהו (כמו הקפצה לחוג/תנועת נוער, עזרה בשיעורי בית וכו')</t>
+  </si>
+  <si>
+    <t>היום אמא שלי עזרה לי במשהו (כמו הקפצה לחוג/תנועת נוער, עזרה בשיעורי בית וכו')</t>
+  </si>
+  <si>
+    <t>מאז הסקר האחרון, שיתפתי את אבא שלי ברגשות/תחושות שלי (שאני שמח / עצוב / כועס / עצבני / שקרה לי משהו מרגש היום)</t>
+  </si>
+  <si>
+    <t>מאז הסקר האחרון, שיתפתי את אמא שלי ברגשות/תחושות שלי (שאני שמח / עצוב / כועס / עצבני / שקרה לי משהו מרגש היום)</t>
   </si>
 </sst>
 </file>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F683BF62-4417-43F4-ADCE-01CD126760AF}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,7 +716,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -761,103 +761,103 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
         <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,7 +870,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -894,282 +894,282 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
         <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
         <v>12</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C52" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" t="s">
         <v>25</v>
-      </c>
-      <c r="C54" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>